<commit_message>
Added the rest of the team photos
</commit_message>
<xml_diff>
--- a/PI-2023-24_Self-Assessment.xlsx
+++ b/PI-2023-24_Self-Assessment.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fernando\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3361817-A403-445D-B1E0-6841317BC92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12432" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -18,7 +24,7 @@
   <definedNames>
     <definedName name="ItemEval">[1]!Table2[ItemEval]</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,6 +36,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -494,7 +502,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
@@ -1224,169 +1232,9 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percentagem" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1432,7 +1280,7 @@
             <xdr14:cNvPr id="7" name="Ink 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{84EA9176-AD5B-1E48-B9F9-F07080AA6832}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84EA9176-AD5B-1E48-B9F9-F07080AA6832}"/>
                 </a:ext>
               </a:extLst>
             </xdr14:cNvPr>
@@ -1497,7 +1345,7 @@
             <xdr14:cNvPr id="14" name="Ink 13">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C11775C-AEBD-3D40-A3A9-CC45ED1B07E2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C11775C-AEBD-3D40-A3A9-CC45ED1B07E2}"/>
                 </a:ext>
               </a:extLst>
             </xdr14:cNvPr>
@@ -1546,7 +1394,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Instructions"/>
@@ -1659,7 +1507,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1711,7 +1559,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1905,48 +1753,48 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="5.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="19" width="7.8984375" customWidth="1"/>
+    <col min="4" max="19" width="7.875" customWidth="1"/>
     <col min="20" max="20" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>137</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1955,13 +1803,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:20" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:20" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="E8" s="65" t="s">
@@ -1983,7 +1831,7 @@
       <c r="S8" s="66"/>
       <c r="T8" s="67"/>
     </row>
-    <row r="9" spans="1:20" ht="105.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" ht="105.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="42">
@@ -2050,7 +1898,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="62" t="s">
         <v>6</v>
       </c>
@@ -2087,7 +1935,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="63"/>
       <c r="C11" s="8">
         <v>1230929</v>
@@ -2122,7 +1970,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="63"/>
       <c r="C12" s="8">
         <v>1231170</v>
@@ -2157,7 +2005,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="63"/>
       <c r="C13" s="8">
         <v>1230481</v>
@@ -2192,7 +2040,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="63"/>
       <c r="C14" s="8">
         <v>1221018</v>
@@ -2227,7 +2075,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="63"/>
       <c r="C15" s="8" t="s">
         <v>7</v>
@@ -2252,7 +2100,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="63"/>
       <c r="C16" s="8" t="s">
         <v>8</v>
@@ -2277,7 +2125,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="63"/>
       <c r="C17" s="8" t="s">
         <v>9</v>
@@ -2302,7 +2150,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="63"/>
       <c r="C18" s="8" t="s">
         <v>10</v>
@@ -2327,7 +2175,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="63"/>
       <c r="C19" s="8" t="s">
         <v>11</v>
@@ -2352,7 +2200,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="63"/>
       <c r="C20" s="8" t="s">
         <v>12</v>
@@ -2377,7 +2225,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="63"/>
       <c r="C21" s="8" t="s">
         <v>13</v>
@@ -2402,7 +2250,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="63"/>
       <c r="C22" s="8" t="s">
         <v>14</v>
@@ -2427,7 +2275,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="63"/>
       <c r="C23" s="8" t="s">
         <v>15</v>
@@ -2452,7 +2300,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="64"/>
       <c r="C24" s="40" t="s">
         <v>16</v>
@@ -2477,7 +2325,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="45" t="s">
         <v>5</v>
@@ -2544,27 +2392,27 @@
       </c>
       <c r="S25" s="53"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0</v>
       </c>
@@ -2572,7 +2420,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2580,7 +2428,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2</v>
       </c>
@@ -2588,7 +2436,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2596,7 +2444,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2604,7 +2452,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>5</v>
       </c>
@@ -2618,7 +2466,7 @@
     <mergeCell ref="E8:T8"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:R24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:R24" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$31:$A$36</formula1>
     </dataValidation>
   </dataValidations>
@@ -2628,29 +2476,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A7" zoomScale="61" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.09765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="20.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" customWidth="1"/>
     <col min="5" max="10" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="30" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
         <v>28</v>
       </c>
@@ -2682,7 +2530,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="63"/>
       <c r="B4" s="71"/>
       <c r="C4" s="71"/>
@@ -2706,7 +2554,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="63"/>
       <c r="B5" s="71"/>
       <c r="C5" s="71"/>
@@ -2730,7 +2578,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>1</v>
       </c>
@@ -2738,7 +2586,7 @@
         <v>1221018</v>
       </c>
       <c r="C6" s="29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" s="60"/>
       <c r="E6" s="31" t="s">
@@ -2760,7 +2608,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>2</v>
       </c>
@@ -2768,7 +2616,7 @@
         <v>1221018</v>
       </c>
       <c r="C7" s="29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D7" s="60"/>
       <c r="E7" s="14" t="s">
@@ -2790,7 +2638,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <v>3</v>
       </c>
@@ -2798,7 +2646,7 @@
         <v>1230929</v>
       </c>
       <c r="C8" s="29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D8" s="60"/>
       <c r="E8" s="14" t="s">
@@ -2820,7 +2668,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>4</v>
       </c>
@@ -2850,7 +2698,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>5</v>
       </c>
@@ -2880,7 +2728,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <v>6</v>
       </c>
@@ -2888,7 +2736,7 @@
         <v>1231170</v>
       </c>
       <c r="C11" s="29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D11" s="60"/>
       <c r="E11" s="14" t="s">
@@ -2910,7 +2758,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>7</v>
       </c>
@@ -2918,7 +2766,7 @@
         <v>1231151</v>
       </c>
       <c r="C12" s="29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12" s="60"/>
       <c r="E12" s="14" t="s">
@@ -2940,7 +2788,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>8</v>
       </c>
@@ -2948,7 +2796,7 @@
         <v>1231151</v>
       </c>
       <c r="C13" s="29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D13" s="60"/>
       <c r="E13" s="14" t="s">
@@ -2970,10 +2818,16 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="14"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
+    <row r="14" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="14">
+        <v>9</v>
+      </c>
+      <c r="B14" s="29">
+        <v>1230481</v>
+      </c>
+      <c r="C14" s="29">
+        <v>4</v>
+      </c>
       <c r="D14" s="60"/>
       <c r="E14" s="14" t="s">
         <v>38</v>
@@ -2994,10 +2848,16 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="14"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
+    <row r="15" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="14">
+        <v>10</v>
+      </c>
+      <c r="B15" s="29">
+        <v>1230929</v>
+      </c>
+      <c r="C15" s="29">
+        <v>4</v>
+      </c>
       <c r="D15" s="60"/>
       <c r="E15" s="14" t="s">
         <v>38</v>
@@ -3018,10 +2878,16 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
+    <row r="16" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="14">
+        <v>11</v>
+      </c>
+      <c r="B16" s="29">
+        <v>1231151</v>
+      </c>
+      <c r="C16" s="29">
+        <v>4</v>
+      </c>
       <c r="D16" s="60"/>
       <c r="E16" s="14" t="s">
         <v>38</v>
@@ -3042,10 +2908,16 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
+    <row r="17" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="14">
+        <v>12</v>
+      </c>
+      <c r="B17" s="29">
+        <v>1231170</v>
+      </c>
+      <c r="C17" s="29">
+        <v>4</v>
+      </c>
       <c r="D17" s="60"/>
       <c r="E17" s="14" t="s">
         <v>38</v>
@@ -3066,10 +2938,16 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="14"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
+    <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
+        <v>13</v>
+      </c>
+      <c r="B18" s="29">
+        <v>1231151</v>
+      </c>
+      <c r="C18" s="29">
+        <v>4</v>
+      </c>
       <c r="D18" s="60"/>
       <c r="E18" s="14" t="s">
         <v>38</v>
@@ -3090,10 +2968,16 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
+    <row r="19" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="14">
+        <v>14</v>
+      </c>
+      <c r="B19" s="29">
+        <v>1231151</v>
+      </c>
+      <c r="C19" s="29">
+        <v>4</v>
+      </c>
       <c r="D19" s="60"/>
       <c r="E19" s="14" t="s">
         <v>38</v>
@@ -3114,7 +2998,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
@@ -3138,7 +3022,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
@@ -3162,7 +3046,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
@@ -3186,7 +3070,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
@@ -3210,7 +3094,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>
@@ -3234,7 +3118,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
       <c r="B25" s="54"/>
       <c r="C25" s="54"/>
@@ -3265,96 +3149,16 @@
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="A3:A5"/>
   </mergeCells>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="expression" dxfId="16" priority="14" stopIfTrue="1">
+  <conditionalFormatting sqref="E6:J25">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>$C6=E$3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F6">
-    <cfRule type="expression" dxfId="15" priority="15" stopIfTrue="1">
-      <formula>$C6=F$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="expression" dxfId="14" priority="16" stopIfTrue="1">
-      <formula>$C6=G$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H6">
-    <cfRule type="expression" dxfId="13" priority="17" stopIfTrue="1">
-      <formula>$C6=H$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I6">
-    <cfRule type="expression" dxfId="12" priority="21" stopIfTrue="1">
-      <formula>$C6=I$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J6">
-    <cfRule type="expression" dxfId="11" priority="22" stopIfTrue="1">
-      <formula>$C6=J$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E7:E17">
-    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
-      <formula>$C7=E$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F7:F17">
-    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
-      <formula>$C7=F$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G7:G17">
-    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
-      <formula>$C7=G$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H7:H17">
-    <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
-      <formula>$C7=H$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I7:I17">
-    <cfRule type="expression" dxfId="6" priority="12" stopIfTrue="1">
-      <formula>$C7=I$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E18:E25">
-    <cfRule type="expression" dxfId="5" priority="2" stopIfTrue="1">
-      <formula>$C18=E$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F18:F25">
-    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
-      <formula>$C18=F$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G18:G25">
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
-      <formula>$C18=G$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H18:H25">
-    <cfRule type="expression" dxfId="2" priority="5" stopIfTrue="1">
-      <formula>$C18=H$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18:I25">
-    <cfRule type="expression" dxfId="1" priority="6" stopIfTrue="1">
-      <formula>$C18=I$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J7:J25">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
-      <formula>$C7=J$3</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18:C25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20:C25" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$E$40:$J$40</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C19" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>$E$3:$J$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -3362,7 +3166,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>'Group and Self Assessment'!$C$10:$C$24</xm:f>
           </x14:formula1>
@@ -3375,32 +3179,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.8984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="17" width="5.59765625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="17" width="5.625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="16.375" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17.5" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.375" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="7.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.8984375" style="1"/>
+    <col min="26" max="26" width="8.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="7.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>47</v>
       </c>
@@ -3419,8 +3223,8 @@
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
     </row>
-    <row r="2" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>48</v>
       </c>
@@ -3521,7 +3325,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="63" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>50</v>
       </c>
@@ -3578,7 +3382,7 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="15"/>
     </row>
-    <row r="5" spans="1:26" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>57</v>
       </c>
@@ -3635,7 +3439,7 @@
       <c r="Y5" s="7"/>
       <c r="Z5" s="15"/>
     </row>
-    <row r="6" spans="1:26" ht="78" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>64</v>
       </c>
@@ -3692,7 +3496,7 @@
       <c r="Y6" s="7"/>
       <c r="Z6" s="15"/>
     </row>
-    <row r="7" spans="1:26" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>70</v>
       </c>
@@ -3739,7 +3543,7 @@
       <c r="Y7" s="7"/>
       <c r="Z7" s="15"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>46</v>
       </c>
@@ -3817,7 +3621,7 @@
       <c r="Y8" s="7"/>
       <c r="Z8" s="15"/>
     </row>
-    <row r="9" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>76</v>
       </c>
@@ -3892,13 +3696,13 @@
       <c r="Y9" s="23"/>
       <c r="Z9" s="16"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:Q7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:Q7" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>$S$3:$X$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -3907,30 +3711,30 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.8984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="17" width="5.59765625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="17" width="5.625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="16.375" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="20.59765625" style="1" customWidth="1"/>
+    <col min="22" max="24" width="20.625" style="1" customWidth="1"/>
     <col min="25" max="25" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="7.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.8984375" style="1"/>
+    <col min="26" max="26" width="8.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="7.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>77</v>
       </c>
@@ -3949,7 +3753,7 @@
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
     </row>
-    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>48</v>
       </c>
@@ -4050,7 +3854,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="144.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>78</v>
       </c>
@@ -4058,19 +3862,19 @@
         <v>0.1</v>
       </c>
       <c r="C4" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F4" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G4" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H4" s="25"/>
       <c r="I4" s="25"/>
@@ -4084,7 +3888,7 @@
       <c r="Q4" s="25"/>
       <c r="R4" s="55">
         <f t="shared" ref="R4:R7" si="0">AVERAGE(C4:Q4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S4" s="59" t="s">
         <v>79</v>
@@ -4107,7 +3911,7 @@
       <c r="Y4" s="56"/>
       <c r="Z4" s="15"/>
     </row>
-    <row r="5" spans="1:26" ht="101.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>85</v>
       </c>
@@ -4164,7 +3968,7 @@
       <c r="Y5" s="56"/>
       <c r="Z5" s="15"/>
     </row>
-    <row r="6" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>92</v>
       </c>
@@ -4221,7 +4025,7 @@
       <c r="Y6" s="56"/>
       <c r="Z6" s="15"/>
     </row>
-    <row r="7" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>99</v>
       </c>
@@ -4278,7 +4082,7 @@
       <c r="Y7" s="56"/>
       <c r="Z7" s="15"/>
     </row>
-    <row r="8" spans="1:26" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="63" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>105</v>
       </c>
@@ -4286,19 +4090,19 @@
         <v>0.1</v>
       </c>
       <c r="C8" s="25">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D8" s="25">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E8" s="25">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F8" s="25">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G8" s="25">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
@@ -4312,7 +4116,7 @@
       <c r="Q8" s="25"/>
       <c r="R8" s="55">
         <f t="shared" ref="R8:R12" si="1">AVERAGE(C8:Q8)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="S8" s="59" t="s">
         <v>93</v>
@@ -4335,7 +4139,7 @@
       <c r="Y8" s="56"/>
       <c r="Z8" s="15"/>
     </row>
-    <row r="9" spans="1:26" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="63" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>111</v>
       </c>
@@ -4343,19 +4147,19 @@
         <v>0.05</v>
       </c>
       <c r="C9" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E9" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F9" s="25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G9" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H9" s="25"/>
       <c r="I9" s="25"/>
@@ -4369,7 +4173,7 @@
       <c r="Q9" s="25"/>
       <c r="R9" s="55">
         <f t="shared" ref="R9:R11" si="2">AVERAGE(C9:Q9)</f>
-        <v>3.2</v>
+        <v>4.2</v>
       </c>
       <c r="S9" s="59" t="s">
         <v>112</v>
@@ -4388,7 +4192,7 @@
       <c r="Y9" s="56"/>
       <c r="Z9" s="15"/>
     </row>
-    <row r="10" spans="1:26" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>116</v>
       </c>
@@ -4396,19 +4200,19 @@
         <v>0.1</v>
       </c>
       <c r="C10" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D10" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E10" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F10" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G10" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H10" s="25"/>
       <c r="I10" s="25"/>
@@ -4422,7 +4226,7 @@
       <c r="Q10" s="25"/>
       <c r="R10" s="55">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S10" s="59" t="s">
         <v>112</v>
@@ -4445,18 +4249,28 @@
       <c r="Y10" s="56"/>
       <c r="Z10" s="15"/>
     </row>
-    <row r="11" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>122</v>
       </c>
       <c r="B11" s="17">
         <v>0.1</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
+      <c r="C11" s="25">
+        <v>3</v>
+      </c>
+      <c r="D11" s="25">
+        <v>3</v>
+      </c>
+      <c r="E11" s="25">
+        <v>3</v>
+      </c>
+      <c r="F11" s="25">
+        <v>3</v>
+      </c>
+      <c r="G11" s="25">
+        <v>3</v>
+      </c>
       <c r="H11" s="25"/>
       <c r="I11" s="25"/>
       <c r="J11" s="25"/>
@@ -4467,9 +4281,9 @@
       <c r="O11" s="25"/>
       <c r="P11" s="25"/>
       <c r="Q11" s="25"/>
-      <c r="R11" s="55" t="e">
+      <c r="R11" s="55">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>3</v>
       </c>
       <c r="S11" s="59" t="s">
         <v>112</v>
@@ -4492,7 +4306,7 @@
       <c r="Y11" s="56"/>
       <c r="Z11" s="15"/>
     </row>
-    <row r="12" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>128</v>
       </c>
@@ -4539,7 +4353,7 @@
       <c r="Y12" s="56"/>
       <c r="Z12" s="15"/>
     </row>
-    <row r="13" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>129</v>
       </c>
@@ -4586,7 +4400,7 @@
       <c r="Y13" s="56"/>
       <c r="Z13" s="15"/>
     </row>
-    <row r="14" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>136</v>
       </c>
@@ -4633,7 +4447,7 @@
       <c r="Y14" s="56"/>
       <c r="Z14" s="15"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>46</v>
       </c>
@@ -4643,23 +4457,23 @@
       </c>
       <c r="C15" s="7">
         <f>SUMPRODUCT(C4:C14,$B$4:$B$14)</f>
-        <v>1.8500000000000003</v>
+        <v>2.5999999999999996</v>
       </c>
       <c r="D15" s="7">
         <f t="shared" ref="D15:Q15" si="4">SUMPRODUCT(D4:D14,$B$4:$B$14)</f>
-        <v>1.8500000000000003</v>
+        <v>2.5999999999999996</v>
       </c>
       <c r="E15" s="7">
         <f t="shared" si="4"/>
-        <v>1.8500000000000003</v>
+        <v>2.5999999999999996</v>
       </c>
       <c r="F15" s="7">
         <f t="shared" si="4"/>
-        <v>1.9000000000000001</v>
+        <v>2.6500000000000004</v>
       </c>
       <c r="G15" s="7">
         <f t="shared" si="4"/>
-        <v>1.8500000000000003</v>
+        <v>2.5999999999999996</v>
       </c>
       <c r="H15" s="7">
         <f t="shared" si="4"/>
@@ -4711,30 +4525,30 @@
       <c r="Y15" s="7"/>
       <c r="Z15" s="15"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>76</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="23">
         <f>C15/5*20</f>
-        <v>7.4000000000000012</v>
+        <v>10.399999999999999</v>
       </c>
       <c r="D16" s="23">
         <f t="shared" ref="D16:Q16" si="5">D15/5*20</f>
-        <v>7.4000000000000012</v>
+        <v>10.399999999999999</v>
       </c>
       <c r="E16" s="23">
         <f t="shared" si="5"/>
-        <v>7.4000000000000012</v>
+        <v>10.399999999999999</v>
       </c>
       <c r="F16" s="23">
         <f t="shared" si="5"/>
-        <v>7.6</v>
+        <v>10.600000000000001</v>
       </c>
       <c r="G16" s="23">
         <f t="shared" si="5"/>
-        <v>7.4000000000000012</v>
+        <v>10.399999999999999</v>
       </c>
       <c r="H16" s="23">
         <f t="shared" si="5"/>
@@ -4786,12 +4600,12 @@
       <c r="Y16" s="23"/>
       <c r="Z16" s="16"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:Q14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:Q14" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>$S$3:$X$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -4810,6 +4624,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005836243B3C47804EAF5FFDD9F066FCC7" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d21ddf3f0b128e39c9d770c8c903166">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0326308c339679ad994635f2c691325" ns2:_="">
     <xsd:import namespace="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
@@ -4993,12 +4813,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
   <ds:schemaRefs>
@@ -5008,6 +4822,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23B77F7C-EE47-4FBD-B078-6536C1487A1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5023,20 +4853,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>